<commit_message>
Update Data Dictionary - carprices.xlsx
</commit_message>
<xml_diff>
--- a/Data Dictionary - carprices.xlsx
+++ b/Data Dictionary - carprices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Linear Regression\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\Class\Spring 2023\COGS 209\Project Proposal\Car_Prediction_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC03834B-F7DC-40BB-B20F-34C63615719D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>Car_ID</t>
-  </si>
-  <si>
-    <t>carCompany</t>
   </si>
   <si>
     <t>fueltype</t>
@@ -207,11 +205,14 @@
   <si>
     <t>Stroke or volume inside the engine (Numeric)</t>
   </si>
+  <si>
+    <t>carName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,6 +489,40 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,41 +541,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -856,11 +857,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F2:N32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="L21" sqref="L21:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -876,456 +877,483 @@
   <sheetData>
     <row r="2" spans="7:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="7:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="18"/>
     </row>
     <row r="5" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="8">
+      <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="14">
-        <v>2</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16" t="s">
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-    </row>
-    <row r="7" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="14">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16" t="s">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-    </row>
-    <row r="8" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="14">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16" t="s">
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-    </row>
-    <row r="9" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="14">
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="4">
+        <v>6</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16" t="s">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-    </row>
-    <row r="10" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="14">
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="4">
+        <v>7</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16" t="s">
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-    </row>
-    <row r="11" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="14">
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <v>8</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16" t="s">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-    </row>
-    <row r="12" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="14">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="4">
+        <v>9</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-    </row>
-    <row r="13" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="14">
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="4">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16" t="s">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="4">
+        <v>11</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="4">
+        <v>12</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="4">
+        <v>13</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="4">
+        <v>14</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="4">
+        <v>15</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-    </row>
-    <row r="14" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="14">
-        <v>10</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-    </row>
-    <row r="15" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="14">
-        <v>11</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-    </row>
-    <row r="16" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="14">
-        <v>12</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="14">
-        <v>13</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-    </row>
-    <row r="18" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G18" s="14">
-        <v>14</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="17" t="s">
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="4">
+        <v>16</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="4">
+        <v>17</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="18"/>
-      <c r="N18" s="19"/>
-    </row>
-    <row r="19" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="14">
-        <v>15</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-    </row>
-    <row r="20" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G20" s="14">
-        <v>16</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16" t="s">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="4">
+        <v>18</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-    </row>
-    <row r="21" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="14">
-        <v>17</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16" t="s">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="4">
+        <v>19</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-    </row>
-    <row r="22" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="14">
-        <v>18</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-    </row>
-    <row r="23" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="14">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="4">
+        <v>20</v>
+      </c>
+      <c r="H24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16" t="s">
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="4">
+        <v>21</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="4">
+        <v>22</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-    </row>
-    <row r="24" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="14">
-        <v>20</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-    </row>
-    <row r="25" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="14">
-        <v>21</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-    </row>
-    <row r="26" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="14">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="4">
+        <v>23</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16" t="s">
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-    </row>
-    <row r="27" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="14">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="4">
+        <v>24</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="16" t="s">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-    </row>
-    <row r="28" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="14">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="4">
+        <v>25</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16" t="s">
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="4">
+        <v>26</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-    </row>
-    <row r="29" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="14">
-        <v>25</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-    </row>
-    <row r="30" spans="7:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="14">
-        <v>26</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
     </row>
     <row r="31" spans="7:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="7:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N32" s="7" t="s">
-        <v>39</v>
+      <c r="N32" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="L18:N18"/>
@@ -1342,38 +1370,11 @@
     <mergeCell ref="H24:K24"/>
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L30:N30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>